<commit_message>
Projektmanagement - Assignment 5 Template hochgeladen und vorbefüllt
</commit_message>
<xml_diff>
--- a/01_Projektmanagement/Anforderungsliste_LHGrundlage.xlsx
+++ b/01_Projektmanagement/Anforderungsliste_LHGrundlage.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ec6dd0bf820af39d/Development/RTW/01_Projektmanagement/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gchri\OneDrive\Development\RTW\01_Projektmanagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="0138E53DE8D533E384D787A1C6DDF303826A3E06" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7536" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,9 +23,9 @@
   </definedNames>
   <calcPr calcId="171027" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Użytkownik Microsoft Office — Widok osobisty" guid="{386D5F1C-3504-2248-AD9B-E2C4C58AAAFA}" mergeInterval="0" personalView="1" windowWidth="1440" windowHeight="618" activeSheetId="1"/>
+    <customWorkbookView name="Chris G - Persönliche Ansicht" guid="{54DE4394-48B3-4927-9148-8B961F019B6C}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
     <customWorkbookView name="gchri - Persönliche Ansicht" guid="{9E52B96B-A190-465D-B01A-58BD3EAF76E3}" mergeInterval="0" personalView="1" maximized="1" xWindow="-9" yWindow="-9" windowWidth="2178" windowHeight="1408" activeSheetId="1"/>
-    <customWorkbookView name="Chris G - Persönliche Ansicht" guid="{54DE4394-48B3-4927-9148-8B961F019B6C}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
-    <customWorkbookView name="Użytkownik Microsoft Office — Widok osobisty" guid="{386D5F1C-3504-2248-AD9B-E2C4C58AAAFA}" mergeInterval="0" personalView="1" windowWidth="1440" windowHeight="618" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -4347,8 +4348,8 @@
   <autoFilter ref="A4:J45" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <dataConsolidate/>
   <customSheetViews>
-    <customSheetView guid="{9E52B96B-A190-465D-B01A-58BD3EAF76E3}" scale="140" showAutoFilter="1">
-      <selection activeCell="G44" sqref="G44"/>
+    <customSheetView guid="{386D5F1C-3504-2248-AD9B-E2C4C58AAAFA}" scale="140" showAutoFilter="1" topLeftCell="B23">
+      <selection activeCell="G35" sqref="G35"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
       <autoFilter ref="A4:J44" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
@@ -4359,8 +4360,8 @@
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
       <autoFilter ref="A4:J44" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
-    <customSheetView guid="{386D5F1C-3504-2248-AD9B-E2C4C58AAAFA}" scale="140" showAutoFilter="1" topLeftCell="B23">
-      <selection activeCell="G35" sqref="G35"/>
+    <customSheetView guid="{9E52B96B-A190-465D-B01A-58BD3EAF76E3}" scale="140" showAutoFilter="1">
+      <selection activeCell="G44" sqref="G44"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
       <autoFilter ref="A4:J44" xr:uid="{00000000-0000-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Raspberry pi und Motoren inMohne Baugruppe eingefügt
</commit_message>
<xml_diff>
--- a/01_Projektmanagement/Anforderungsliste_LHGrundlage.xlsx
+++ b/01_Projektmanagement/Anforderungsliste_LHGrundlage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gchri\OneDrive\Development\RTW\01_Projektmanagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="0138E53DE8D533E384D787A1C6DDF303826A3E06" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="0138E53DE8D533E384D787A1C6DDF303826A3E06" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{E4667759-EE27-4266-8F17-D1DA276134FE}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7536" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,9 +23,9 @@
   </definedNames>
   <calcPr calcId="171027" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="gchri - Persönliche Ansicht" guid="{9E52B96B-A190-465D-B01A-58BD3EAF76E3}" mergeInterval="0" personalView="1" maximized="1" xWindow="-9" yWindow="-9" windowWidth="2178" windowHeight="1408" activeSheetId="1"/>
+    <customWorkbookView name="Chris G - Persönliche Ansicht" guid="{54DE4394-48B3-4927-9148-8B961F019B6C}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
     <customWorkbookView name="Użytkownik Microsoft Office — Widok osobisty" guid="{386D5F1C-3504-2248-AD9B-E2C4C58AAAFA}" mergeInterval="0" personalView="1" windowWidth="1440" windowHeight="618" activeSheetId="1"/>
-    <customWorkbookView name="Chris G - Persönliche Ansicht" guid="{54DE4394-48B3-4927-9148-8B961F019B6C}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
-    <customWorkbookView name="gchri - Persönliche Ansicht" guid="{9E52B96B-A190-465D-B01A-58BD3EAF76E3}" mergeInterval="0" personalView="1" maximized="1" xWindow="-9" yWindow="-9" windowWidth="2178" windowHeight="1408" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>Anforderungsliste des Projekts</t>
   </si>
@@ -143,6 +143,54 @@
   </si>
   <si>
     <t>Muss ohne Schäden überstanden werden</t>
+  </si>
+  <si>
+    <t>Sandfahren gerade aus</t>
+  </si>
+  <si>
+    <t>Stufen überwinden 10-60cm</t>
+  </si>
+  <si>
+    <t>Wasser und Sand überstehen gerade aus</t>
+  </si>
+  <si>
+    <t>Hindernisse umfahren 40x40 rot</t>
+  </si>
+  <si>
+    <t>Beastmode = Alles schaffen</t>
+  </si>
+  <si>
+    <t>Randbedingung</t>
+  </si>
+  <si>
+    <t>Pflicht</t>
+  </si>
+  <si>
+    <t>autonom fliegen</t>
+  </si>
+  <si>
+    <t>Fahrmodus</t>
+  </si>
+  <si>
+    <t>Drohne muss die meiste zeit fahren</t>
+  </si>
+  <si>
+    <t>Mit Kamera und Ultraschallsensor</t>
+  </si>
+  <si>
+    <t>Hindernisserkennung + Zielanflug</t>
+  </si>
+  <si>
+    <t>Drohne muss wasserdicht sein</t>
+  </si>
+  <si>
+    <t>Notstop</t>
+  </si>
+  <si>
+    <t>im notfall dünnes seil, anglerschnurr</t>
+  </si>
+  <si>
+    <t>Drohen (Mohne) fertigen</t>
   </si>
 </sst>
 </file>
@@ -713,7 +761,7 @@
   <dimension ref="A1:U308"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" outlineLevelCol="1"/>
@@ -751,7 +799,7 @@
       </c>
       <c r="C2" s="6">
         <f ca="1">TODAY()</f>
-        <v>43119</v>
+        <v>43120</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -815,8 +863,12 @@
       <c r="C5" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
+      <c r="D5" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>22</v>
+      </c>
       <c r="F5" s="33"/>
       <c r="G5" s="27"/>
       <c r="H5" s="14"/>
@@ -825,11 +877,19 @@
       <c r="K5" s="11"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="11"/>
-      <c r="B6" s="12"/>
+      <c r="A6" s="11">
+        <v>2</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>16</v>
+      </c>
       <c r="C6" s="12"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
+      <c r="D6" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>22</v>
+      </c>
       <c r="F6" s="33"/>
       <c r="G6" s="28"/>
       <c r="H6" s="15"/>
@@ -838,10 +898,16 @@
       <c r="K6" s="11"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="11"/>
-      <c r="B7" s="12"/>
+      <c r="A7" s="11">
+        <v>3</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>17</v>
+      </c>
       <c r="C7" s="12"/>
-      <c r="D7" s="32"/>
+      <c r="D7" s="32" t="s">
+        <v>21</v>
+      </c>
       <c r="E7" s="32"/>
       <c r="F7" s="33"/>
       <c r="G7" s="28"/>
@@ -850,11 +916,19 @@
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
     </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="11"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="32"/>
+    <row r="8" spans="1:11" ht="28.8">
+      <c r="A8" s="11">
+        <v>4</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>21</v>
+      </c>
       <c r="E8" s="32"/>
       <c r="F8" s="33"/>
       <c r="G8" s="28"/>
@@ -863,11 +937,17 @@
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
     </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="11"/>
-      <c r="B9" s="12"/>
+    <row r="9" spans="1:11" ht="28.8">
+      <c r="A9" s="11">
+        <v>5</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>19</v>
+      </c>
       <c r="C9" s="12"/>
-      <c r="D9" s="32"/>
+      <c r="D9" s="32" t="s">
+        <v>21</v>
+      </c>
       <c r="E9" s="32"/>
       <c r="F9" s="33"/>
       <c r="G9" s="28"/>
@@ -877,10 +957,16 @@
       <c r="K9" s="11"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="11"/>
-      <c r="B10" s="17"/>
+      <c r="A10" s="11">
+        <v>6</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>20</v>
+      </c>
       <c r="C10" s="17"/>
-      <c r="D10" s="34"/>
+      <c r="D10" s="34" t="s">
+        <v>21</v>
+      </c>
       <c r="E10" s="34"/>
       <c r="F10" s="33"/>
       <c r="G10" s="29"/>
@@ -890,8 +976,12 @@
       <c r="K10" s="16"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="11"/>
-      <c r="B11" s="12"/>
+      <c r="A11" s="11">
+        <v>7</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>31</v>
+      </c>
       <c r="C11" s="12"/>
       <c r="D11" s="32"/>
       <c r="E11" s="32"/>
@@ -903,8 +993,12 @@
       <c r="K11" s="11"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="11"/>
-      <c r="B12" s="12"/>
+      <c r="A12" s="11">
+        <v>8</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>23</v>
+      </c>
       <c r="C12" s="12"/>
       <c r="D12" s="32"/>
       <c r="E12" s="32"/>
@@ -916,9 +1010,15 @@
       <c r="K12" s="11"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="11"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
+      <c r="A13" s="11">
+        <v>9</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>25</v>
+      </c>
       <c r="D13" s="32"/>
       <c r="E13" s="32"/>
       <c r="F13" s="33"/>
@@ -928,10 +1028,16 @@
       <c r="J13" s="11"/>
       <c r="K13" s="11"/>
     </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="11"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
+    <row r="14" spans="1:11" ht="28.8">
+      <c r="A14" s="11">
+        <v>10</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="D14" s="32"/>
       <c r="E14" s="32"/>
       <c r="F14" s="33"/>
@@ -942,9 +1048,15 @@
       <c r="K14" s="11"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="11"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
+      <c r="A15" s="11">
+        <v>11</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>30</v>
+      </c>
       <c r="D15" s="32"/>
       <c r="E15" s="32"/>
       <c r="F15" s="33"/>
@@ -4348,8 +4460,8 @@
   <autoFilter ref="A4:J45" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <dataConsolidate/>
   <customSheetViews>
-    <customSheetView guid="{386D5F1C-3504-2248-AD9B-E2C4C58AAAFA}" scale="140" showAutoFilter="1" topLeftCell="B23">
-      <selection activeCell="G35" sqref="G35"/>
+    <customSheetView guid="{9E52B96B-A190-465D-B01A-58BD3EAF76E3}" scale="140" showAutoFilter="1">
+      <selection activeCell="G44" sqref="G44"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
       <autoFilter ref="A4:J44" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
@@ -4360,8 +4472,8 @@
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
       <autoFilter ref="A4:J44" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
-    <customSheetView guid="{9E52B96B-A190-465D-B01A-58BD3EAF76E3}" scale="140" showAutoFilter="1">
-      <selection activeCell="G44" sqref="G44"/>
+    <customSheetView guid="{386D5F1C-3504-2248-AD9B-E2C4C58AAAFA}" scale="140" showAutoFilter="1" topLeftCell="B23">
+      <selection activeCell="G35" sqref="G35"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
       <autoFilter ref="A4:J44" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
@@ -4389,7 +4501,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Nicht vorgesehner Wert" error="Ihre Eingabe ist Ungültig._x000a_Bitte nutzen Sie die Dropdown Funktionalität des Feldes um alle möglichen Eingabewerte zu sehen und direkt einzugeben." sqref="D5:D78" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Nicht vorgesehner Wert" error="Ihre Eingabe ist Ungültig._x000a_Bitte nutzen Sie die Dropdown Funktionalität des Feldes um alle möglichen Eingabewerte zu sehen und direkt einzugeben." sqref="D6:D78 D5" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Funktional,Qualität,Randbedingung"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Nicht vorgesehner Wert" error="Ihre Eingabe ist Ungültig._x000a_Bitte nutzen Sie die Dropdown Funktionalität des Feldes um alle möglichen Eingabewerte zu sehen und direkt einzugeben." sqref="E5:E78" xr:uid="{00000000-0002-0000-0000-000001000000}">

</xml_diff>

<commit_message>
Kompletten Projektbericht überarbeitet, Diagramme und Grafiken angepasst.
</commit_message>
<xml_diff>
--- a/01_Projektmanagement/Anforderungsliste_LHGrundlage.xlsx
+++ b/01_Projektmanagement/Anforderungsliste_LHGrundlage.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\OneDrive\Development\RTW\01_Projektmanagement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gchri\OneDrive\Development\RTW\01_Projektmanagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="42" documentId="0138E53DE8D533E384D787A1C6DDF303826A3E06" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{400C287C-2F74-453F-8286-56876BD38550}"/>
@@ -23,9 +23,9 @@
   </definedNames>
   <calcPr calcId="171027" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="gchri - Persönliche Ansicht" guid="{9E52B96B-A190-465D-B01A-58BD3EAF76E3}" mergeInterval="0" personalView="1" maximized="1" xWindow="-9" yWindow="-9" windowWidth="2178" windowHeight="1408" activeSheetId="1"/>
+    <customWorkbookView name="Chris G - Persönliche Ansicht" guid="{54DE4394-48B3-4927-9148-8B961F019B6C}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
     <customWorkbookView name="Użytkownik Microsoft Office — Widok osobisty" guid="{386D5F1C-3504-2248-AD9B-E2C4C58AAAFA}" mergeInterval="0" personalView="1" windowWidth="1440" windowHeight="618" activeSheetId="1"/>
-    <customWorkbookView name="Chris G - Persönliche Ansicht" guid="{54DE4394-48B3-4927-9148-8B961F019B6C}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
-    <customWorkbookView name="gchri - Persönliche Ansicht" guid="{9E52B96B-A190-465D-B01A-58BD3EAF76E3}" mergeInterval="0" personalView="1" maximized="1" xWindow="-9" yWindow="-9" windowWidth="2178" windowHeight="1408" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -796,7 +796,7 @@
       </c>
       <c r="C2" s="6">
         <f ca="1">TODAY()</f>
-        <v>43156</v>
+        <v>43169</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -4452,8 +4452,8 @@
   <autoFilter ref="A4:J45" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <dataConsolidate/>
   <customSheetViews>
-    <customSheetView guid="{386D5F1C-3504-2248-AD9B-E2C4C58AAAFA}" scale="140" showAutoFilter="1" topLeftCell="B23">
-      <selection activeCell="G35" sqref="G35"/>
+    <customSheetView guid="{9E52B96B-A190-465D-B01A-58BD3EAF76E3}" scale="140" showAutoFilter="1">
+      <selection activeCell="G44" sqref="G44"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
       <autoFilter ref="A4:J44" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
@@ -4464,8 +4464,8 @@
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
       <autoFilter ref="A4:J44" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
-    <customSheetView guid="{9E52B96B-A190-465D-B01A-58BD3EAF76E3}" scale="140" showAutoFilter="1">
-      <selection activeCell="G44" sqref="G44"/>
+    <customSheetView guid="{386D5F1C-3504-2248-AD9B-E2C4C58AAAFA}" scale="140" showAutoFilter="1" topLeftCell="B23">
+      <selection activeCell="G35" sqref="G35"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
       <autoFilter ref="A4:J44" xr:uid="{00000000-0000-0000-0000-000000000000}"/>

</xml_diff>